<commit_message>
Add a number when XLS columns have identical names
</commit_message>
<xml_diff>
--- a/tests/testdata.xlsx
+++ b/tests/testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpasternak/Programowanie/xlsx2postgresql/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD2B6490-016A-544A-AADC-FE4FEADCBF0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3512880A-BF60-4040-82D1-4055E8177574}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -394,6 +394,47 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="8"/>
+        </left>
+        <right style="thin">
+          <color indexed="8"/>
+        </right>
+        <top style="thin">
+          <color indexed="8"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="8"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
       <fill>
         <patternFill patternType="solid">
@@ -681,14 +722,96 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor indexed="9"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="8"/>
+        </left>
+        <right style="thin">
+          <color indexed="8"/>
+        </right>
+        <top style="thin">
+          <color indexed="8"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="8"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="8"/>
+        </left>
+        <right style="thin">
+          <color indexed="8"/>
+        </right>
+        <top style="thin">
+          <color indexed="8"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="8"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="8"/>
@@ -845,129 +968,6 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="8"/>
-        </left>
-        <right style="thin">
-          <color indexed="8"/>
-        </right>
-        <top style="thin">
-          <color indexed="8"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="8"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="8"/>
-        </left>
-        <right style="thin">
-          <color indexed="8"/>
-        </right>
-        <top style="thin">
-          <color indexed="8"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="8"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="9"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="8"/>
-        </left>
-        <right style="thin">
-          <color indexed="8"/>
-        </right>
-        <top style="thin">
-          <color indexed="8"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="8"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
       <fill>
         <patternFill patternType="solid">
@@ -1084,13 +1084,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color indexed="8"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="medium">
           <color indexed="8"/>
         </top>
@@ -1122,6 +1115,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="8"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1239,7 +1239,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A8:S16" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" headerRowBorderDxfId="20" tableBorderDxfId="21" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A8:S16" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="A8:S16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="L.p." dataDxfId="18"/>
@@ -1253,14 +1253,14 @@
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Element operacji - Czas trwania (w minutach)" dataDxfId="10"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Personel uczestniczący - Imiona" dataDxfId="9"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Personel uczestniczący - Nazwisko" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Jednostka zlecająca - Nazwa" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Personel uczestniczący - KOD" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Personel uczestniczący - Rola - Kod" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Element operacji - Typ elementu leczenia" dataDxfId="4"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Dane pacjenta - Identyfikator pacjenta (MIP)" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Dane pacjenta - Data urodzenia" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Procedury medyczne - Kod procedury" dataDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Procedury medyczne - Nazwa" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Jednostka zlecająca - Nazwa" dataDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Personel uczestniczący - KOD" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Personel uczestniczący - Rola - Kod" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Element operacji - Typ elementu leczenia" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Dane pacjenta - Identyfikator pacjenta (MIP)" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Dane pacjenta - Data urodzenia" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Procedury medyczne - Kod procedury" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Procedury medyczne - Nazwa" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1565,8 +1565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>